<commit_message>
Readme edit and updates
</commit_message>
<xml_diff>
--- a/docs/validation/user_story_testing.xlsx
+++ b/docs/validation/user_story_testing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="151">
   <si>
     <t>User Stories Link</t>
   </si>
@@ -94,12 +94,6 @@
 Given that new/returning user visits
 When they scroll down
 Then they can see excerpts of different posts with which they can understand the type of content the website provides and are given an option to select any post to visit</t>
-  </si>
-  <si>
-    <t>Acceptance Criteria 5:
-Given that new/returning user visits
-When they wish to search a post using keyword
-Then they can type in keyword in Search input field and can arrive at the post with matching keyword</t>
   </si>
   <si>
     <t>https://github.com/RoshnaVakkeel/Little_Learners_Lab_Logs/issues/4</t>
@@ -532,12 +526,99 @@
   <si>
     <t>Alerts Messages</t>
   </si>
+  <si>
+    <t>Acceptance Criteria 4:
+Given that the user who visits personal page
+When they are signed in
+Then they can see an update profile option which allows them to update or even delete their account</t>
+  </si>
+  <si>
+    <t>My Page Profile section</t>
+  </si>
+  <si>
+    <t>My Page Lab Logs section</t>
+  </si>
+  <si>
+    <t>https://github.com/RoshnaVakkeel/Little_Learners_Lab_Logs/issues/20</t>
+  </si>
+  <si>
+    <t>USER STORY US16: Sorting and Searching #20</t>
+  </si>
+  <si>
+    <t>As a Site user I can see distinct search criteria so that I can sort and find the log posts easily</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria 1:
+Given that new/returning user visits the Lab Logs page
+When they can see a dropdown menu with options of selecting different titles
+Then they can select a log post directly from the menu list and don't need to scroll down and find the posts</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria 2:
+Given that new/returning user is on a lab log post
+When they can see a category tag
+Then they can identify what is the difficulty level of the experiment</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria 3:
+Given that new/returning user visits the Lab Logs nav link
+When they can see a dropdown menu with options in an alphabetical order
+Then they can select a log post easily</t>
+  </si>
+  <si>
+    <t>Lab Logs page, button</t>
+  </si>
+  <si>
+    <t>Lab Logs posts, Homepage, my-page and lab-logs page</t>
+  </si>
+  <si>
+    <t>https://github.com/RoshnaVakkeel/Little_Learners_Lab_Logs/issues/22</t>
+  </si>
+  <si>
+    <t>US17: Profile page #22</t>
+  </si>
+  <si>
+    <t>As a user, I can see profile update option, so that I can update my profile info</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria 1:
+Given that the signed in user is on their personal page
+When they can a profile update button
+Then they can update or delete their profile</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria 2:
+Given that the signed in user edits their profile
+When they click submit
+Then they receive a message and the updates would reflect on their personal page</t>
+  </si>
+  <si>
+    <t>Update Profile page, Update Profile button - my-page</t>
+  </si>
+  <si>
+    <t>Update Profile page, Profile section - my-page</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria 4:
+Given that new/returning user visits
+When they wish to search a post using keyword
+Then they can type in keyword in Search input field and can arrive at the post with matching keyword</t>
+  </si>
+  <si>
+    <t>https://github.com/RoshnaVakkeel/Little_Learners_Lab_Logs#sort-and-search</t>
+  </si>
+  <si>
+    <t>https://github.com/RoshnaVakkeel/Little_Learners_Lab_Logs#all-lab-logs</t>
+  </si>
+  <si>
+    <t>https://github.com/RoshnaVakkeel/Little_Learners_Lab_Logs#profile-update</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -575,6 +656,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -600,7 +688,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -624,6 +712,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -919,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -953,10 +1044,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="75">
@@ -976,10 +1067,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="75">
@@ -991,10 +1082,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="75">
@@ -1005,10 +1096,10 @@
         <v>9</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1031,10 +1122,10 @@
         <v>9</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60">
@@ -1045,13 +1136,13 @@
         <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="60">
+    </row>
+    <row r="8" spans="1:7" ht="75">
       <c r="D8" s="3" t="s">
         <v>17</v>
       </c>
@@ -1059,10 +1150,10 @@
         <v>9</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="90">
@@ -1073,75 +1164,61 @@
         <v>9</v>
       </c>
       <c r="F9" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="75">
-      <c r="D10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="90">
+      <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="75">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="75">
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="75">
       <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1149,53 +1226,53 @@
     </row>
     <row r="15" spans="1:7" ht="75">
       <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60">
       <c r="D16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="60">
       <c r="D17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1203,53 +1280,53 @@
     </row>
     <row r="19" spans="1:7" ht="90">
       <c r="A19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="D19" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="60">
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="75">
       <c r="D21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1257,39 +1334,39 @@
     </row>
     <row r="23" spans="1:7" ht="75">
       <c r="A23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="75">
+      <c r="D24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="60">
-      <c r="D24" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="E24" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1297,67 +1374,67 @@
     </row>
     <row r="26" spans="1:7" ht="75">
       <c r="A26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="90">
+      <c r="D27" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="G26" s="2" t="s">
+      <c r="E27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="75">
-      <c r="D27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="75">
       <c r="D28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="75">
+      <c r="D29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="60">
-      <c r="D29" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="E29" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F29" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1365,133 +1442,144 @@
     </row>
     <row r="31" spans="1:7" ht="90">
       <c r="A31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="E31" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="75">
       <c r="D32" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="75">
       <c r="D33" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F33" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="E34" s="7"/>
+    </row>
+    <row r="34" spans="1:7" ht="75">
+      <c r="D34" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="90">
       <c r="A35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="E35" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="60">
       <c r="D36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="90">
+      <c r="D37" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="5" t="s">
+      <c r="E37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="75">
-      <c r="D37" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:7" ht="75">
+    <row r="39" spans="1:7" ht="90">
       <c r="A39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="E39" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F39" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1501,39 +1589,39 @@
     </row>
     <row r="41" spans="1:7" ht="90">
       <c r="A41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="E41" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="90">
+      <c r="D42" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G41" s="2" t="s">
+      <c r="E42" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="75">
-      <c r="D42" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="G42" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1541,25 +1629,25 @@
     </row>
     <row r="44" spans="1:7" ht="90">
       <c r="A44" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="E44" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F44" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1567,92 +1655,214 @@
     </row>
     <row r="46" spans="1:7" ht="105">
       <c r="A46" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="E46" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:7" ht="75">
+    <row r="48" spans="1:7" ht="105">
       <c r="A48" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="E48" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F48" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:7" ht="75">
+    <row r="50" spans="1:7" ht="90">
       <c r="A50" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="E50" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F50" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="60">
+    </row>
+    <row r="51" spans="1:7" ht="75">
       <c r="D51" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E51" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="G51" s="2" t="s">
-        <v>104</v>
-      </c>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="90">
+      <c r="A53" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="75">
+      <c r="D54" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="75">
+      <c r="D55" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="75">
+      <c r="D56" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="E57" s="7"/>
+    </row>
+    <row r="59" spans="1:7" ht="60">
+      <c r="A59" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="75">
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="E61" s="7"/>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="E62" s="7"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="E63" s="7"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="E64" s="7"/>
+    </row>
+    <row r="65" spans="5:5">
+      <c r="E65" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1678,7 +1888,7 @@
     <hyperlink ref="G4" r:id="rId20" location="getting-started"/>
     <hyperlink ref="G8" r:id="rId21" location="hero-image"/>
     <hyperlink ref="G9" r:id="rId22" location="lab-logs"/>
-    <hyperlink ref="G10" r:id="rId23" location="search-button"/>
+    <hyperlink ref="G56" r:id="rId23" location="search-button"/>
     <hyperlink ref="G11" r:id="rId24" location="lab-logs"/>
     <hyperlink ref="G12" r:id="rId25" location="lab-logs_x000a_" display="https://github.com/RoshnaVakkeel/Little_Learners_Lab_Logs#lab-logs_x000a_"/>
     <hyperlink ref="G13" r:id="rId26" location="log-details"/>
@@ -1708,9 +1918,17 @@
     <hyperlink ref="G50" r:id="rId50" location="log-details"/>
     <hyperlink ref="G51" r:id="rId51" location="log-details"/>
     <hyperlink ref="G23" r:id="rId52" location="alert-messages"/>
+    <hyperlink ref="G34" r:id="rId53"/>
+    <hyperlink ref="A53" r:id="rId54"/>
+    <hyperlink ref="A59" r:id="rId55"/>
+    <hyperlink ref="G53" r:id="rId56" location="sort-and-search"/>
+    <hyperlink ref="G54" r:id="rId57" location="all-lab-logs"/>
+    <hyperlink ref="G55" r:id="rId58" location="sort-and-search"/>
+    <hyperlink ref="G59" r:id="rId59" location="profile-update"/>
+    <hyperlink ref="G60" r:id="rId60" location="my-page"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId53"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId61"/>
 </worksheet>
 </file>
 

</xml_diff>